<commit_message>
Site updated: 2024-07-27 14:43:04
</commit_message>
<xml_diff>
--- a/doc/2号线三队用户积分信息表模板202401111951.xlsx
+++ b/doc/2号线三队用户积分信息表模板202401111951.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>姓名</t>
   </si>
@@ -56,6 +56,9 @@
     <t>驾驶资格</t>
   </si>
   <si>
+    <t>是否队长</t>
+  </si>
+  <si>
     <t>李晓骑</t>
   </si>
   <si>
@@ -78,6 +81,9 @@
   </si>
   <si>
     <t>一条线驾驶资格</t>
+  </si>
+  <si>
+    <t>是</t>
   </si>
   <si>
     <t>史珺</t>
@@ -105,8 +111,16 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
-    <font>
+  <fonts count="24">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -610,147 +624,156 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1278,137 +1301,148 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="14.6666666666667" customWidth="1"/>
-    <col min="4" max="4" width="15.3333333333333" customWidth="1"/>
-    <col min="5" max="5" width="11.6666666666667" customWidth="1"/>
-    <col min="6" max="6" width="10.7777777777778" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="14.1111111111111" customWidth="1"/>
-    <col min="9" max="9" width="20.5555555555556" customWidth="1"/>
+    <col min="1" max="2" width="8.88888888888889" style="2"/>
+    <col min="3" max="3" width="14.6666666666667" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.3333333333333" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.6666666666667" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.7777777777778" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20" style="2" customWidth="1"/>
+    <col min="8" max="8" width="14.1111111111111" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16.4444444444444" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.1111111111111" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" t="s">
+    <row r="1" s="1" customFormat="1" spans="1:10">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" ht="15.6" customHeight="1" spans="1:9">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2">
+    <row r="2" ht="15.6" customHeight="1" spans="1:10">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="5">
         <v>600313</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2" s="5" t="s">
         <v>16</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" ht="15.6" customHeight="1" spans="1:9">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="5">
         <v>601187</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" ht="15.6" customHeight="1" spans="1:10">
+      <c r="A4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="5">
+        <v>601190</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" ht="15.6" customHeight="1" spans="1:9">
-      <c r="A4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="2">
-        <v>601190</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" ht="15.6" customHeight="1"/>

</xml_diff>